<commit_message>
sped up unix c version by 2x
</commit_message>
<xml_diff>
--- a/p2/webstats_one_thread_per_file/Webstats.xlsx
+++ b/p2/webstats_one_thread_per_file/Webstats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18520" yWindow="0" windowWidth="18400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="18620" yWindow="0" windowWidth="18400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -781,7 +781,7 @@
         <v>15</v>
       </c>
       <c r="B23">
-        <v>8.7479999999999993</v>
+        <v>4.4859999999999998</v>
       </c>
       <c r="C23">
         <v>2587176</v>

</xml_diff>